<commit_message>
Update Risk analysis - PID (Probability Impact Diagram) diagram, RAID.xlsx
</commit_message>
<xml_diff>
--- a/Project Management/Risk analysis - PID (Probability Impact Diagram) diagram, RAID.xlsx
+++ b/Project Management/Risk analysis - PID (Probability Impact Diagram) diagram, RAID.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/dominic2_pennycook_live_uwe_ac_uk/Documents/Year 3/GDIP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\UNI\Year 3\GDIP\GDIP_ROBOT\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ACCA625-5C3C-4D66-B12F-1C53F619B987}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878E66CE-07A9-4046-8909-F4CB2044CF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PID" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -77,9 +77,6 @@
     <t xml:space="preserve">Product isn't acceptable to Investors </t>
   </si>
   <si>
-    <t>Develop a robust Verification and Validation Plan</t>
-  </si>
-  <si>
     <t>Negligible</t>
   </si>
   <si>
@@ -255,13 +252,16 @@
   </si>
   <si>
     <t>Outline necessary health and saftely plan fopr customers, limmit the potential speed nad torque of the arm</t>
+  </si>
+  <si>
+    <t>Develop a robust Verification and Validation Plan, UPDATE - Plan was created lowering the liklily hood</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,7 +544,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -832,7 +832,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -842,11 +842,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6623F95-A144-420B-860F-B2F0655A949A}">
   <dimension ref="C1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -862,8 +862,8 @@
     <col min="16" max="16" width="120.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16" ht="15.75" thickBot="1"/>
-    <row r="2" spans="3:16">
+    <row r="1" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -892,7 +892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="3:16">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
@@ -937,7 +937,7 @@
       </c>
       <c r="P3" s="21"/>
     </row>
-    <row r="4" spans="3:16">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
@@ -978,7 +978,7 @@
       </c>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="3:16">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1014,7 +1014,7 @@
       <c r="O5" s="20"/>
       <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="3:16">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1051,19 +1051,19 @@
         <v>5</v>
       </c>
       <c r="N6" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O6" s="20">
         <f>N6*M6</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P6" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="3:16">
-      <c r="C7" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1089,10 +1089,10 @@
         <v>5</v>
       </c>
       <c r="K7" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="25" t="s">
         <v>16</v>
-      </c>
-      <c r="L7" s="25" t="s">
-        <v>17</v>
       </c>
       <c r="M7" s="20">
         <v>3</v>
@@ -1105,10 +1105,10 @@
         <v>9</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="3:16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="E8">
         <v>1</v>
@@ -1126,7 +1126,7 @@
         <v>5</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
@@ -1134,31 +1134,31 @@
       <c r="O8" s="20"/>
       <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="3:16" ht="15.75" thickBot="1">
+    <row r="9" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="K9" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="24" t="s">
+      <c r="L9" s="25" t="s">
         <v>25</v>
-      </c>
-      <c r="L9" s="25" t="s">
-        <v>26</v>
       </c>
       <c r="M9" s="20">
         <v>5</v>
@@ -1171,15 +1171,15 @@
         <v>5</v>
       </c>
       <c r="P9" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="3:16" ht="15.75" thickBot="1">
-      <c r="K10" s="24" t="s">
+      <c r="L10" s="25" t="s">
         <v>28</v>
-      </c>
-      <c r="L10" s="25" t="s">
-        <v>29</v>
       </c>
       <c r="M10" s="20">
         <v>4</v>
@@ -1192,22 +1192,22 @@
         <v>4</v>
       </c>
       <c r="P10" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="39" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="3:16">
-      <c r="C11" s="39" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
       <c r="F11" s="40"/>
       <c r="G11" s="41"/>
       <c r="K11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="25" t="s">
         <v>32</v>
-      </c>
-      <c r="L11" s="25" t="s">
-        <v>33</v>
       </c>
       <c r="M11" s="20">
         <v>4</v>
@@ -1219,21 +1219,21 @@
         <v>4</v>
       </c>
       <c r="P11" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="3:16">
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="31" t="s">
         <v>35</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>36</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="32"/>
       <c r="K12" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
@@ -1241,21 +1241,21 @@
       <c r="O12" s="20"/>
       <c r="P12" s="21"/>
     </row>
-    <row r="13" spans="3:16">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="33" t="s">
         <v>38</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>39</v>
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="33"/>
       <c r="G13" s="34"/>
       <c r="K13" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="25" t="s">
         <v>40</v>
-      </c>
-      <c r="L13" s="25" t="s">
-        <v>41</v>
       </c>
       <c r="M13" s="20">
         <v>4</v>
@@ -1268,24 +1268,24 @@
         <v>4</v>
       </c>
       <c r="P13" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="3:16">
-      <c r="C14" s="14" t="s">
+      <c r="D14" s="35" t="s">
         <v>43</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>44</v>
       </c>
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
       <c r="G14" s="36"/>
       <c r="K14" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="25" t="s">
         <v>45</v>
-      </c>
-      <c r="L14" s="25" t="s">
-        <v>46</v>
       </c>
       <c r="M14" s="20">
         <v>4</v>
@@ -1298,21 +1298,21 @@
         <v>4</v>
       </c>
       <c r="P14" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="3:16" ht="15.75" thickBot="1">
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="37" t="s">
         <v>48</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>49</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37"/>
       <c r="G15" s="38"/>
       <c r="K15" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
@@ -1320,12 +1320,12 @@
       <c r="O15" s="20"/>
       <c r="P15" s="21"/>
     </row>
-    <row r="16" spans="3:16" ht="30">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="K16" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="25" t="s">
         <v>51</v>
-      </c>
-      <c r="L16" s="25" t="s">
-        <v>52</v>
       </c>
       <c r="M16" s="20">
         <v>3</v>
@@ -1338,15 +1338,15 @@
         <v>3</v>
       </c>
       <c r="P16" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K17" s="24" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="11:16">
-      <c r="K17" s="24" t="s">
+      <c r="L17" s="25" t="s">
         <v>54</v>
-      </c>
-      <c r="L17" s="25" t="s">
-        <v>55</v>
       </c>
       <c r="M17" s="20">
         <v>3</v>
@@ -1359,15 +1359,15 @@
         <v>3</v>
       </c>
       <c r="P17" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K18" s="24" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="11:16">
-      <c r="K18" s="24" t="s">
+      <c r="L18" s="25" t="s">
         <v>57</v>
-      </c>
-      <c r="L18" s="25" t="s">
-        <v>58</v>
       </c>
       <c r="M18" s="20">
         <v>4</v>
@@ -1380,12 +1380,12 @@
         <v>4</v>
       </c>
       <c r="P18" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K19" s="22" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="11:16">
-      <c r="K19" s="22" t="s">
-        <v>60</v>
       </c>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
@@ -1393,12 +1393,12 @@
       <c r="O19" s="20"/>
       <c r="P19" s="21"/>
     </row>
-    <row r="20" spans="11:16">
+    <row r="20" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K20" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="L20" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="M20" s="20">
         <v>5</v>
@@ -1411,15 +1411,15 @@
         <v>5</v>
       </c>
       <c r="P20" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K21" s="24" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="11:16">
-      <c r="K21" s="24" t="s">
+      <c r="L21" s="25" t="s">
         <v>64</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>65</v>
       </c>
       <c r="M21" s="20">
         <v>3</v>
@@ -1432,12 +1432,12 @@
         <v>12</v>
       </c>
       <c r="P21" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K22" s="22" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="11:16">
-      <c r="K22" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
@@ -1445,12 +1445,12 @@
       <c r="O22" s="20"/>
       <c r="P22" s="21"/>
     </row>
-    <row r="23" spans="11:16">
+    <row r="23" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K23" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="L23" s="25" t="s">
         <v>68</v>
-      </c>
-      <c r="L23" s="25" t="s">
-        <v>69</v>
       </c>
       <c r="M23" s="20">
         <v>5</v>
@@ -1463,15 +1463,15 @@
         <v>10</v>
       </c>
       <c r="P23" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="28" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="11:16" ht="15.75" thickBot="1">
-      <c r="K24" s="28" t="s">
+      <c r="L24" s="29" t="s">
         <v>71</v>
-      </c>
-      <c r="L24" s="29" t="s">
-        <v>72</v>
       </c>
       <c r="M24" s="23">
         <v>4</v>
@@ -1484,10 +1484,10 @@
         <v>12</v>
       </c>
       <c r="P24" s="30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="11:16">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="11:16" x14ac:dyDescent="0.25">
       <c r="M26">
         <v>0</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="11:16">
+    <row r="27" spans="11:16" x14ac:dyDescent="0.25">
       <c r="M27">
         <v>0</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="11:16">
+    <row r="28" spans="11:16" x14ac:dyDescent="0.25">
       <c r="M28">
         <v>0</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="11:16">
+    <row r="29" spans="11:16" x14ac:dyDescent="0.25">
       <c r="M29">
         <v>0</v>
       </c>

</xml_diff>